<commit_message>
updating my pres copy with FRED data overview
</commit_message>
<xml_diff>
--- a/Enrollment-Completions-Unemployment Chart.xlsx
+++ b/Enrollment-Completions-Unemployment Chart.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carter\Desktop\Project 1\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FF966E04-FAFE-45C4-B376-6C7D5EABB981}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{418DB576-5DEB-46A5-8813-44B3F2EA7513}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" firstSheet="2" activeTab="2" xr2:uid="{170E097B-D646-4A64-9597-7E0C22C8C3E2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" activeTab="1" xr2:uid="{170E097B-D646-4A64-9597-7E0C22C8C3E2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="enrollmentByYear_for_CombinedPl" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId3"/>
+    <sheet name="enrollmentByYear_for_CombinedPl" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId2"/>
+    <sheet name="Unemployment vs. Enroll - Lag" sheetId="6" r:id="rId3"/>
     <sheet name="Regression Output Lag" sheetId="9" r:id="rId4"/>
     <sheet name="Regression Output" sheetId="7" r:id="rId5"/>
   </sheets>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
   <si>
     <t>Jobless Claims Annual Rate of Change</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Standard Residuals</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -1961,7 +1964,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$12</c:f>
+              <c:f>'Unemployment vs. Enroll - Lag'!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2198,7 +2201,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$12</c:f>
+              <c:f>'Unemployment vs. Enroll - Lag'!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2240,7 +2243,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$3:$B$13</c:f>
+              <c:f>'Unemployment vs. Enroll - Lag'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2300,7 +2303,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$12</c:f>
+              <c:f>'Unemployment vs. Enroll - Lag'!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2538,46 +2541,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$13</c:f>
+              <c:f>'Unemployment vs. Enroll - Lag'!$C$2:$C$13</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>-9.8039215686274495E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.26086956521739102</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.60344827586206895</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.2258064516128997E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-7.2916666666666602E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-8.9887640449438297E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-8.6419753086419693E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.162162162162162</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.14516129032257999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-7.5471698113207392E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.10204081632653</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2669,7 +2636,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2781,52 +2748,16 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$13</c:f>
+              <c:f>'Unemployment vs. Enroll - Lag'!$C$2:$C$13</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>-9.8039215686274495E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.26086956521739102</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.60344827586206895</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.2258064516128997E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-7.2916666666666602E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-8.9887640449438297E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-8.6419753086419693E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.162162162162162</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.14516129032257999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-7.5471698113207392E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.10204081632653</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$13</c:f>
+              <c:f>'Unemployment vs. Enroll - Lag'!$B$1:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2889,46 +2820,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$13</c:f>
+              <c:f>'Unemployment vs. Enroll - Lag'!$C$2:$C$13</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>-9.8039215686274495E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.26086956521739102</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.60344827586206895</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.2258064516128997E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-7.2916666666666602E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-8.9887640449438297E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-8.6419753086419693E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.162162162162162</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.14516129032257999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-7.5471698113207392E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.10204081632653</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3020,7 +2915,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4132,23 +4027,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3BF9B9-FA1D-454C-BCE3-37975A72B66D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129B9969-730A-4BB3-8361-5364EC299E5F}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:O14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4857,200 +4740,514 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009078FF-EFA5-4D06-8FC8-155E46149E78}">
-  <dimension ref="A1:D13"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A509193-0C6F-4DCC-A729-62FC5E30E1BA}">
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:C18"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="32.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2006</v>
+      </c>
+      <c r="B2" s="2">
+        <v>8.3266313464631647E-3</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2">
+        <v>2008</v>
+      </c>
+      <c r="E2" s="2">
+        <v>-1.5834987564743219E-2</v>
+      </c>
+      <c r="G2">
+        <v>2006</v>
+      </c>
+      <c r="H2" s="2">
+        <v>-4.0025729343901695E-2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>-9.8039215686274495E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f t="shared" ref="A3:A13" si="0">A2+1</f>
+        <v>2007</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.4175312229361525E-2</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3">
+        <v>2009</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.1486564811165465</v>
+      </c>
+      <c r="G3">
+        <v>2007</v>
+      </c>
+      <c r="H3" s="2">
+        <v>-5.2696422781800534E-2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>2008</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.3416891024645059E-2</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4">
+        <v>2010</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.23130487435664548</v>
+      </c>
+      <c r="G4">
+        <v>2008</v>
+      </c>
+      <c r="H4" s="2">
+        <v>-1.5834987564743219E-2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.26086956521739102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>2009</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5.7879158241936457E-2</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5">
+        <v>2011</v>
+      </c>
+      <c r="E5" s="2">
+        <v>-0.22327678059175482</v>
+      </c>
+      <c r="G5">
+        <v>2009</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.1486564811165465</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.60344827586206895</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>2010</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5.6689791194729722E-2</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6">
+        <v>2012</v>
+      </c>
+      <c r="E6" s="2">
+        <v>-3.904271484045263E-3</v>
+      </c>
+      <c r="G6">
+        <v>2010</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.23130487435664548</v>
+      </c>
+      <c r="J6" s="1">
+        <v>3.2258064516128997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.6382979384981464E-2</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7">
+        <v>2013</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-0.16341447912032037</v>
+      </c>
+      <c r="G7">
+        <v>2011</v>
+      </c>
+      <c r="H7" s="2">
+        <v>-0.22327678059175482</v>
+      </c>
+      <c r="J7" s="1">
+        <v>-7.2916666666666602E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2.50353355879529E-5</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8">
+        <v>2014</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-2.3020817504938451E-2</v>
+      </c>
+      <c r="G8">
+        <v>2012</v>
+      </c>
+      <c r="H8" s="2">
+        <v>-3.904271484045263E-3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>-8.9887640449438297E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-1.3916479078157185E-2</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9">
+        <v>2015</v>
+      </c>
+      <c r="E9" s="2">
+        <v>-3.6368820799958512E-2</v>
+      </c>
+      <c r="G9">
+        <v>2013</v>
+      </c>
+      <c r="H9" s="2">
+        <v>-0.16341447912032037</v>
+      </c>
+      <c r="J9" s="1">
+        <v>-8.6419753086419693E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3.0969971731826806E-3</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10">
+        <v>2016</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3.8279442621186766E-2</v>
+      </c>
+      <c r="G10">
+        <v>2014</v>
+      </c>
+      <c r="H10" s="2">
+        <v>-2.3020817504938451E-2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>-0.162162162162162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+      <c r="B11" s="2">
+        <v>-8.2065752990195806E-3</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11">
+        <v>2017</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2.5338756898204418E-2</v>
+      </c>
+      <c r="G11">
+        <v>2015</v>
+      </c>
+      <c r="H11" s="2">
+        <v>-3.6368820799958512E-2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-0.14516129032257999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="G12">
+        <v>2016</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3.8279442621186766E-2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>-7.5471698113207392E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="G13">
+        <v>2017</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2.5338756898204418E-2</v>
+      </c>
+      <c r="J13" s="1">
+        <v>-0.10204081632653</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009078FF-EFA5-4D06-8FC8-155E46149E78}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.26953125" customWidth="1"/>
+    <col min="5" max="5" width="33.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
+      <c r="B1" t="s">
+        <v>13</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
+        <v>2007</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.4175312229361525E-2</v>
+      </c>
+      <c r="D2">
         <v>2006</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-4.0025729343901695E-2</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>-9.8039215686274495E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
+        <v>2008</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2.3416891024645059E-2</v>
+      </c>
+      <c r="D3">
         <v>2007</v>
       </c>
-      <c r="B3" s="2">
-        <v>1.4175312229361525E-2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>-5.2696422781800534E-2</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
+        <v>2009</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5.7879158241936457E-2</v>
+      </c>
+      <c r="D4">
         <v>2008</v>
       </c>
-      <c r="B4" s="2">
-        <v>2.3416891024645059E-2</v>
-      </c>
-      <c r="C4" s="2">
-        <v>-1.5834987564743219E-2</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>0.26086956521739102</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
+        <v>2010</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5.6689791194729722E-2</v>
+      </c>
+      <c r="D5">
         <v>2009</v>
       </c>
-      <c r="B5" s="2">
-        <v>5.7879158241936457E-2</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.1486564811165465</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>0.60344827586206895</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
+        <v>2011</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.6382979384981464E-2</v>
+      </c>
+      <c r="D6">
         <v>2010</v>
       </c>
-      <c r="B6" s="2">
-        <v>5.6689791194729722E-2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.23130487435664548</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>3.2258064516128997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
+        <v>2012</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.50353355879529E-5</v>
+      </c>
+      <c r="D7">
         <v>2011</v>
       </c>
-      <c r="B7" s="2">
-        <v>2.6382979384981464E-2</v>
-      </c>
-      <c r="C7" s="2">
-        <v>-0.22327678059175482</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>-7.2916666666666602E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
+        <v>2013</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-1.3916479078157185E-2</v>
+      </c>
+      <c r="D8">
         <v>2012</v>
       </c>
-      <c r="B8" s="2">
-        <v>2.50353355879529E-5</v>
-      </c>
-      <c r="C8" s="2">
-        <v>-3.904271484045263E-3</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>-8.9887640449438297E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
+        <v>2014</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3.0969971731826806E-3</v>
+      </c>
+      <c r="D9">
         <v>2013</v>
       </c>
-      <c r="B9" s="2">
-        <v>-1.3916479078157185E-2</v>
-      </c>
-      <c r="C9" s="2">
-        <v>-0.16341447912032037</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>-8.6419753086419693E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
+        <v>2015</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-8.2065752990195806E-3</v>
+      </c>
+      <c r="D10">
         <v>2014</v>
       </c>
-      <c r="B10" s="2">
-        <v>3.0969971731826806E-3</v>
-      </c>
-      <c r="C10" s="2">
-        <v>-2.3020817504938451E-2</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>-0.162162162162162</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
+        <v>2016</v>
+      </c>
+      <c r="B11" s="2">
+        <v>-7.1577320288447321E-3</v>
+      </c>
+      <c r="D11">
         <v>2015</v>
       </c>
-      <c r="B11" s="2">
-        <v>-8.2065752990195806E-3</v>
-      </c>
-      <c r="C11" s="2">
-        <v>-3.6368820799958512E-2</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>-0.14516129032257999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
+        <v>2017</v>
+      </c>
+      <c r="B12" s="2">
+        <v>-1.0045048999059003E-2</v>
+      </c>
+      <c r="D12">
         <v>2016</v>
       </c>
-      <c r="B12" s="2">
-        <v>-7.1577320288447321E-3</v>
-      </c>
-      <c r="C12" s="2">
-        <v>3.8279442621186766E-2</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>-7.5471698113207392E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>2017</v>
-      </c>
-      <c r="B13" s="2">
-        <v>-1.0045048999059003E-2</v>
-      </c>
-      <c r="C13" s="2">
-        <v>2.5338756898204418E-2</v>
-      </c>
-      <c r="D13" s="1">
-        <v>-0.10204081632653</v>
-      </c>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>